<commit_message>
fixed a bug in the KNN made earlier today, the final data is named : final_steel_data.xlsx
</commit_message>
<xml_diff>
--- a/Comp/merged_file.xlsx
+++ b/Comp/merged_file.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/vj923_ic_ac_uk/Documents/Imperial/Y2/Steel Challenge/Challenge-2024-2025/Comp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_5799B3F743668A0E62355476585DCE3A87443810" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01D736D9-A4C0-4166-858B-9D0497DB5776}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_5799B3F743668A0E62355476585DCE3A87443810" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1915B754-22BD-420A-8B5D-B2293B1A9FDF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1374,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="M264" sqref="M264"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>